<commit_message>
added PCB models and revise PCB to move DC module on top
</commit_message>
<xml_diff>
--- a/6lowPan/Gerber and BoM/mbed-lowpan-BoM.xlsx
+++ b/6lowPan/Gerber and BoM/mbed-lowpan-BoM.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="210">
   <si>
     <t>Ref</t>
   </si>
@@ -324,9 +324,6 @@
     <t>X1</t>
   </si>
   <si>
-    <t>ESP_EXT, SENSOR-DHT, STM-SWD, STM-USART</t>
-  </si>
-  <si>
     <t>IC1</t>
   </si>
   <si>
@@ -339,12 +336,6 @@
     <t>U$9, U$10, U$11</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
-    <t>U$7</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -661,6 +652,24 @@
   </si>
   <si>
     <t>Andtech</t>
+  </si>
+  <si>
+    <t>Digikey link</t>
+  </si>
+  <si>
+    <t>ESP_EXT, STM-SWD, STM-USART</t>
+  </si>
+  <si>
+    <t>U$17</t>
+  </si>
+  <si>
+    <t>DHT11</t>
+  </si>
+  <si>
+    <t>DHT11 temperature humidity sensor</t>
+  </si>
+  <si>
+    <t>J1, U$7</t>
   </si>
 </sst>
 </file>
@@ -1050,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,21 +1086,21 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>180</v>
-      </c>
-      <c r="B2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C2" t="s">
-        <v>182</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>183</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -1102,13 +1111,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1124,6 +1133,9 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="E4" s="3" t="s">
+        <v>204</v>
+      </c>
       <c r="F4">
         <v>1</v>
       </c>
@@ -1144,7 +1156,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
         <v>24</v>
@@ -1228,7 +1240,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>34</v>
@@ -1250,10 +1262,10 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -1264,13 +1276,13 @@
         <v>77</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1298,13 +1310,13 @@
         <v>67</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F16">
         <v>2</v>
@@ -1315,10 +1327,10 @@
         <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C17" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1335,7 +1347,7 @@
         <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1352,7 +1364,7 @@
         <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="F19">
         <v>2</v>
@@ -1360,7 +1372,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
@@ -1369,7 +1381,7 @@
         <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F20">
         <v>4</v>
@@ -1471,7 +1483,7 @@
         <v>41</v>
       </c>
       <c r="D26" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1567,13 +1579,13 @@
         <v>13</v>
       </c>
       <c r="B32" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C32" t="s">
         <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F32">
         <v>3</v>
@@ -1584,13 +1596,13 @@
         <v>14</v>
       </c>
       <c r="B33" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
         <v>30</v>
       </c>
       <c r="D33" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F33">
         <v>3</v>
@@ -1607,7 +1619,7 @@
         <v>46</v>
       </c>
       <c r="D34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="F34">
         <v>2</v>
@@ -1618,13 +1630,13 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D35" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -1632,7 +1644,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
@@ -1641,7 +1653,7 @@
         <v>49</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F36">
         <v>6</v>
@@ -1649,7 +1661,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B37" t="s">
         <v>45</v>
@@ -1658,7 +1670,7 @@
         <v>46</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F37">
         <v>6</v>
@@ -1675,7 +1687,7 @@
         <v>46</v>
       </c>
       <c r="D38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -1692,7 +1704,7 @@
         <v>46</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="F39">
         <v>3</v>
@@ -1709,7 +1721,7 @@
         <v>46</v>
       </c>
       <c r="D40" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="F40">
         <v>4</v>
@@ -1720,13 +1732,13 @@
         <v>76</v>
       </c>
       <c r="B41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C41" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F41">
         <v>2</v>
@@ -1743,7 +1755,7 @@
         <v>46</v>
       </c>
       <c r="D42" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F42">
         <v>2</v>
@@ -1760,7 +1772,7 @@
         <v>49</v>
       </c>
       <c r="D43" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="F43">
         <v>3</v>
@@ -1768,7 +1780,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B44" t="s">
         <v>39</v>
@@ -1777,7 +1789,7 @@
         <v>40</v>
       </c>
       <c r="D44" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F44">
         <v>6</v>
@@ -1785,7 +1797,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B45" t="s">
         <v>38</v>
@@ -1794,7 +1806,7 @@
         <v>41</v>
       </c>
       <c r="D45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F45">
         <v>4</v>
@@ -1811,7 +1823,7 @@
         <v>41</v>
       </c>
       <c r="D46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F46">
         <v>2</v>
@@ -1819,7 +1831,7 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B47" t="s">
         <v>38</v>
@@ -1828,7 +1840,7 @@
         <v>41</v>
       </c>
       <c r="D47" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F47">
         <v>2</v>
@@ -1845,7 +1857,7 @@
         <v>46</v>
       </c>
       <c r="D48" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F48">
         <v>4</v>
@@ -1862,7 +1874,7 @@
         <v>49</v>
       </c>
       <c r="D49" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -1879,7 +1891,7 @@
         <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F50">
         <v>2</v>
@@ -1887,7 +1899,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B51" t="s">
         <v>45</v>
@@ -1896,7 +1908,7 @@
         <v>46</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F51">
         <v>2</v>
@@ -1904,7 +1916,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B52" t="s">
         <v>48</v>
@@ -1913,7 +1925,7 @@
         <v>49</v>
       </c>
       <c r="D52" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -1924,13 +1936,13 @@
         <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D53" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F53">
         <v>3</v>
@@ -1947,7 +1959,7 @@
         <v>46</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F54">
         <v>3</v>
@@ -1958,13 +1970,13 @@
         <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C55" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -1975,13 +1987,13 @@
         <v>87</v>
       </c>
       <c r="B56" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C56" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D56" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -1992,13 +2004,13 @@
         <v>88</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C57" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D57" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -2006,19 +2018,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B58" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C58" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D58" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2029,16 +2041,16 @@
         <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C59" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D59" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -2049,13 +2061,13 @@
         <v>90</v>
       </c>
       <c r="B60" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C60" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D60" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="F60">
         <v>2</v>
@@ -2066,7 +2078,7 @@
         <v>91</v>
       </c>
       <c r="C61" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2077,13 +2089,13 @@
         <v>92</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D62" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -2094,13 +2106,13 @@
         <v>93</v>
       </c>
       <c r="B63" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C63" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D63" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2108,33 +2120,33 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>94</v>
+        <v>205</v>
       </c>
       <c r="B64" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C64" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D64" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F64">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C65" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D65" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2142,19 +2154,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B66" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C66" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D66" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2162,16 +2174,16 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B67" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D67" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2179,16 +2191,19 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B68" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C68" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D68" t="s">
-        <v>174</v>
+        <v>171</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="F68">
         <v>3</v>
@@ -2196,33 +2211,33 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>99</v>
+        <v>209</v>
       </c>
       <c r="B69" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D69" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B70" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C70" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D70" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2230,16 +2245,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>101</v>
+        <v>188</v>
       </c>
       <c r="B71" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="C71" t="s">
-        <v>177</v>
-      </c>
-      <c r="D71" t="s">
-        <v>176</v>
+        <v>187</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2247,16 +2262,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>190</v>
+      </c>
+      <c r="B72" t="s">
+        <v>189</v>
+      </c>
+      <c r="C72" t="s">
         <v>191</v>
       </c>
-      <c r="B72" t="s">
-        <v>196</v>
-      </c>
-      <c r="C72" t="s">
-        <v>190</v>
-      </c>
       <c r="E72" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2264,16 +2279,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="B73" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="C73" t="s">
-        <v>194</v>
-      </c>
-      <c r="E73" s="3" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -2284,14 +2296,16 @@
     <hyperlink ref="E66" r:id="rId1"/>
     <hyperlink ref="E2" r:id="rId2"/>
     <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E73" r:id="rId4"/>
-    <hyperlink ref="E72" r:id="rId5"/>
+    <hyperlink ref="E72" r:id="rId4"/>
+    <hyperlink ref="E71" r:id="rId5"/>
     <hyperlink ref="E58" r:id="rId6"/>
     <hyperlink ref="E59" r:id="rId7"/>
+    <hyperlink ref="E4" r:id="rId8"/>
+    <hyperlink ref="E68" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
-  <legacyDrawing r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update all PCB design
</commit_message>
<xml_diff>
--- a/6lowPan/Gerber and BoM/mbed-lowpan-BoM.xlsx
+++ b/6lowPan/Gerber and BoM/mbed-lowpan-BoM.xlsx
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update PCB and BoM to use vertical RJ11
</commit_message>
<xml_diff>
--- a/6lowPan/Gerber and BoM/mbed-lowpan-BoM.xlsx
+++ b/6lowPan/Gerber and BoM/mbed-lowpan-BoM.xlsx
@@ -564,9 +564,6 @@
     <t>U$14, U$15, U$16</t>
   </si>
   <si>
-    <t>PY-SMTRJ45-005</t>
-  </si>
-  <si>
     <t>SMT RJ11 4 pin port</t>
   </si>
   <si>
@@ -676,6 +673,9 @@
   </si>
   <si>
     <t>4 pin link</t>
+  </si>
+  <si>
+    <t>RJ11-4P4C-SMT</t>
   </si>
 </sst>
 </file>
@@ -1065,8 +1065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1092,7 +1092,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1100,13 +1100,13 @@
         <v>173</v>
       </c>
       <c r="B2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" t="s">
         <v>174</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" s="3" t="s">
         <v>175</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>176</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -1117,10 +1117,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>161</v>
@@ -1140,7 +1140,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -1157,7 +1157,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F5">
         <v>2</v>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
         <v>23</v>
@@ -1233,7 +1233,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
         <v>30</v>
@@ -1250,7 +1250,7 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
@@ -1264,7 +1264,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>32</v>
@@ -1621,7 +1621,7 @@
         <v>29</v>
       </c>
       <c r="D32" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>161</v>
@@ -1641,7 +1641,7 @@
         <v>29</v>
       </c>
       <c r="D33" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>161</v>
@@ -1686,7 +1686,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B36" t="s">
         <v>46</v>
@@ -1703,7 +1703,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B37" t="s">
         <v>43</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B44" t="s">
         <v>37</v>
@@ -1839,7 +1839,7 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B45" t="s">
         <v>36</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B51" t="s">
         <v>43</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
@@ -2012,13 +2012,13 @@
         <v>84</v>
       </c>
       <c r="B55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C55" t="s">
         <v>137</v>
       </c>
       <c r="D55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>161</v>
@@ -2066,16 +2066,16 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C58" t="s">
         <v>143</v>
       </c>
       <c r="D58" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>161</v>
@@ -2129,10 +2129,10 @@
         <v>149</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2177,7 +2177,7 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B64" t="s">
         <v>158</v>
@@ -2223,7 +2223,7 @@
         <v>163</v>
       </c>
       <c r="D66" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>161</v>
@@ -2271,7 +2271,7 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B69" t="s">
         <v>172</v>
@@ -2305,16 +2305,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B71" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C71" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2322,16 +2322,16 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>185</v>
+      </c>
+      <c r="B72" t="s">
+        <v>184</v>
+      </c>
+      <c r="C72" t="s">
         <v>186</v>
       </c>
-      <c r="B72" t="s">
-        <v>185</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="E72" s="3" t="s">
         <v>187</v>
-      </c>
-      <c r="E72" s="3" t="s">
-        <v>188</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2339,13 +2339,13 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
+        <v>200</v>
+      </c>
+      <c r="B73" t="s">
         <v>201</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>202</v>
-      </c>
-      <c r="C73" t="s">
-        <v>203</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -2354,31 +2354,31 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E66" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
-    <hyperlink ref="E3" r:id="rId3"/>
-    <hyperlink ref="E72" r:id="rId4"/>
-    <hyperlink ref="E71" r:id="rId5"/>
-    <hyperlink ref="E58" r:id="rId6"/>
-    <hyperlink ref="E59" r:id="rId7"/>
-    <hyperlink ref="E4" r:id="rId8"/>
-    <hyperlink ref="E68" r:id="rId9" display="link"/>
-    <hyperlink ref="E11" r:id="rId10"/>
-    <hyperlink ref="E55" r:id="rId11"/>
-    <hyperlink ref="E62" r:id="rId12"/>
-    <hyperlink ref="E64" r:id="rId13"/>
-    <hyperlink ref="E7" r:id="rId14"/>
-    <hyperlink ref="E8" r:id="rId15"/>
-    <hyperlink ref="E9" r:id="rId16"/>
-    <hyperlink ref="E14" r:id="rId17"/>
-    <hyperlink ref="E23" r:id="rId18"/>
-    <hyperlink ref="E25" r:id="rId19"/>
-    <hyperlink ref="E10" r:id="rId20"/>
-    <hyperlink ref="E32" r:id="rId21"/>
-    <hyperlink ref="E33" r:id="rId22"/>
-    <hyperlink ref="E61" r:id="rId23"/>
-    <hyperlink ref="D61" r:id="rId24"/>
-    <hyperlink ref="E57" r:id="rId25"/>
-    <hyperlink ref="E17" r:id="rId26"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E72" r:id="rId3"/>
+    <hyperlink ref="E71" r:id="rId4"/>
+    <hyperlink ref="E58" r:id="rId5"/>
+    <hyperlink ref="E59" r:id="rId6"/>
+    <hyperlink ref="E4" r:id="rId7"/>
+    <hyperlink ref="E68" r:id="rId8" display="link"/>
+    <hyperlink ref="E11" r:id="rId9"/>
+    <hyperlink ref="E55" r:id="rId10"/>
+    <hyperlink ref="E62" r:id="rId11"/>
+    <hyperlink ref="E64" r:id="rId12"/>
+    <hyperlink ref="E7" r:id="rId13"/>
+    <hyperlink ref="E8" r:id="rId14"/>
+    <hyperlink ref="E9" r:id="rId15"/>
+    <hyperlink ref="E14" r:id="rId16"/>
+    <hyperlink ref="E23" r:id="rId17"/>
+    <hyperlink ref="E25" r:id="rId18"/>
+    <hyperlink ref="E10" r:id="rId19"/>
+    <hyperlink ref="E32" r:id="rId20"/>
+    <hyperlink ref="E33" r:id="rId21"/>
+    <hyperlink ref="E61" r:id="rId22"/>
+    <hyperlink ref="D61" r:id="rId23"/>
+    <hyperlink ref="E57" r:id="rId24"/>
+    <hyperlink ref="E17" r:id="rId25"/>
+    <hyperlink ref="E2" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId27"/>

</xml_diff>